<commit_message>
switch from stm to esp
</commit_message>
<xml_diff>
--- a/servo_tester_pca/Лист Microsoft Excel.xlsx
+++ b/servo_tester_pca/Лист Microsoft Excel.xlsx
@@ -436,7 +436,7 @@
   <dimension ref="B3:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +566,7 @@
         <v>11</v>
       </c>
       <c r="G13">
-        <v>300</v>
+        <v>251</v>
       </c>
       <c r="I13">
         <v>135</v>
@@ -618,7 +618,7 @@
         <v>12</v>
       </c>
       <c r="G15">
-        <v>492</v>
+        <v>440</v>
       </c>
       <c r="I15">
         <v>535</v>
@@ -694,10 +694,10 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>300</v>
+        <v>251</v>
       </c>
       <c r="D21">
-        <v>492</v>
+        <v>440</v>
       </c>
       <c r="F21" t="s">
         <v>20</v>

</xml_diff>